<commit_message>
Fix bug in responses.xlsx
</commit_message>
<xml_diff>
--- a/data/Input/Responses.xlsx
+++ b/data/Input/Responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF612CBA-A395-034E-9E6E-319903A4444E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE33DF2-19AE-454D-8623-00D6645074FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,9 +537,6 @@
     <t>Raghavendra</t>
   </si>
   <si>
-    <t>M/W schedule [8:05 - 9:15 a.m.]</t>
-  </si>
-  <si>
     <t>M/W schedule [10:10 - 11:25 a.m.]</t>
   </si>
   <si>
@@ -574,6 +571,9 @@
   </si>
   <si>
     <t>Ding</t>
+  </si>
+  <si>
+    <t>M/W schedule [8:00 - 9:15 a.m.]</t>
   </si>
 </sst>
 </file>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="114" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="114" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1508,19 +1508,19 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>180</v>
+      </c>
+      <c r="R1" t="s">
         <v>168</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>169</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>170</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>171</v>
-      </c>
-      <c r="U1" t="s">
-        <v>172</v>
       </c>
       <c r="V1" t="s">
         <v>16</v>
@@ -2630,10 +2630,10 @@
     </row>
     <row r="52" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" t="s">
         <v>173</v>
-      </c>
-      <c r="C52" t="s">
-        <v>174</v>
       </c>
       <c r="E52" s="2">
         <v>1</v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="53" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E53" s="2">
         <v>1</v>
@@ -2658,10 +2658,10 @@
     </row>
     <row r="54" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E54" s="2">
         <v>2</v>
@@ -2675,10 +2675,10 @@
     </row>
     <row r="55" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>

</xml_diff>